<commit_message>
Updates for first meetup.
</commit_message>
<xml_diff>
--- a/Schedule.xlsx
+++ b/Schedule.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10713"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10814"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jbryer/Dropbox (SPS)/Teaching/DATA661 2022 Fall/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{A5C31DEF-CE9B-2C40-B39D-6BE70AD80811}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1FF223D-AF23-FA42-9D2D-2C23BD897745}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11580" yWindow="5400" windowWidth="28040" windowHeight="17440" xr2:uid="{7F5CD000-6067-3243-B614-D8018D7B2D00}"/>
+    <workbookView xWindow="21880" yWindow="9960" windowWidth="28040" windowHeight="17440" xr2:uid="{7F5CD000-6067-3243-B614-D8018D7B2D00}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,14 +35,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="22">
   <si>
     <t>Week</t>
   </si>
   <si>
-    <t>Week of</t>
-  </si>
-  <si>
     <t>Meetup Topic</t>
   </si>
   <si>
@@ -67,9 +64,6 @@
     <t>Predictive model metrics</t>
   </si>
   <si>
-    <t>Attempt to contribute your first dataset</t>
-  </si>
-  <si>
     <t>R Package Development</t>
   </si>
   <si>
@@ -95,6 +89,19 @@
   </si>
   <si>
     <t>Final class presentation to MSDS community</t>
+  </si>
+  <si>
+    <t>Install the mldash R package (including setting up Python and Java).
+Find your first dataset and try to use it with the mldash package.</t>
+  </si>
+  <si>
+    <t>Attempt to contribute your first model.</t>
+  </si>
+  <si>
+    <t>Meetup</t>
+  </si>
+  <si>
+    <t>8/30/2022 7:00pm</t>
   </si>
 </sst>
 </file>
@@ -143,10 +150,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -464,7 +475,7 @@
   <dimension ref="A1:D16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -478,32 +489,38 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>2</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" s="2">
         <v>1</v>
       </c>
+      <c r="B2" s="4" t="s">
+        <v>21</v>
+      </c>
       <c r="C2" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="D2" s="2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+    </row>
+    <row r="3" spans="1:4" ht="68" x14ac:dyDescent="0.2">
       <c r="A3" s="2">
         <v>2</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
@@ -511,10 +528,10 @@
         <v>3</v>
       </c>
       <c r="C4" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D4" s="2" t="s">
         <v>7</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
@@ -522,10 +539,10 @@
         <v>4</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>10</v>
+        <v>19</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
@@ -533,7 +550,7 @@
         <v>5</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
@@ -541,7 +558,7 @@
         <v>6</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
@@ -549,7 +566,7 @@
         <v>7</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
@@ -557,7 +574,7 @@
         <v>8</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
@@ -565,7 +582,7 @@
         <v>9</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
@@ -573,7 +590,7 @@
         <v>10</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
@@ -581,7 +598,7 @@
         <v>11</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
@@ -589,7 +606,7 @@
         <v>12</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
@@ -597,7 +614,7 @@
         <v>13</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
@@ -605,7 +622,7 @@
         <v>14</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
@@ -613,7 +630,7 @@
         <v>15</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
   </sheetData>

</xml_diff>